<commit_message>
Individual Project Creation and Downloaded Placeholder Things
Updated SPMP and Gantt Chart
</commit_message>
<xml_diff>
--- a/Project Gantt Chart.xlsx
+++ b/Project Gantt Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UnYieldinSpirit\Documents\Towson Work\Fall 2020\COSC 412 Individual\412 Individual Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UnYieldinSpirit\Documents\Towson Work\Fall 2020\COSC 412 Individual\412-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BC1C04-A4B1-4183-AEB1-B0DF2F328A5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59000561-CEF3-436E-8B3C-B707B26F2CD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30255" yWindow="5625" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -453,7 +453,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="157">
   <si>
     <t>[Company Name]</t>
   </si>
@@ -2933,24 +2933,6 @@
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2958,9 +2940,27 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3797,7 +3797,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3825,29 +3825,29 @@
       <c r="E1" s="46"/>
       <c r="F1" s="46"/>
       <c r="I1" s="131"/>
-      <c r="K1" s="169" t="s">
+      <c r="K1" s="163" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="169"/>
-      <c r="M1" s="169"/>
-      <c r="N1" s="169"/>
-      <c r="O1" s="169"/>
-      <c r="P1" s="169"/>
-      <c r="Q1" s="169"/>
-      <c r="R1" s="169"/>
-      <c r="S1" s="169"/>
-      <c r="T1" s="169"/>
-      <c r="U1" s="169"/>
-      <c r="V1" s="169"/>
-      <c r="W1" s="169"/>
-      <c r="X1" s="169"/>
-      <c r="Y1" s="169"/>
-      <c r="Z1" s="169"/>
-      <c r="AA1" s="169"/>
-      <c r="AB1" s="169"/>
-      <c r="AC1" s="169"/>
-      <c r="AD1" s="169"/>
-      <c r="AE1" s="169"/>
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="163"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="163"/>
+      <c r="T1" s="163"/>
+      <c r="U1" s="163"/>
+      <c r="V1" s="163"/>
+      <c r="W1" s="163"/>
+      <c r="X1" s="163"/>
+      <c r="Y1" s="163"/>
+      <c r="Z1" s="163"/>
+      <c r="AA1" s="163"/>
+      <c r="AB1" s="163"/>
+      <c r="AC1" s="163"/>
+      <c r="AD1" s="163"/>
+      <c r="AE1" s="163"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51" t="s">
@@ -3892,11 +3892,11 @@
       <c r="B4" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="171">
+      <c r="C4" s="168">
         <v>44116</v>
       </c>
-      <c r="D4" s="171"/>
-      <c r="E4" s="171"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
       <c r="F4" s="110"/>
       <c r="G4" s="113" t="s">
         <v>76</v>
@@ -3906,180 +3906,180 @@
       </c>
       <c r="I4" s="111"/>
       <c r="J4" s="49"/>
-      <c r="K4" s="163" t="str">
+      <c r="K4" s="165" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="164"/>
-      <c r="M4" s="164"/>
-      <c r="N4" s="164"/>
-      <c r="O4" s="164"/>
-      <c r="P4" s="164"/>
-      <c r="Q4" s="165"/>
-      <c r="R4" s="163" t="str">
+      <c r="L4" s="166"/>
+      <c r="M4" s="166"/>
+      <c r="N4" s="166"/>
+      <c r="O4" s="166"/>
+      <c r="P4" s="166"/>
+      <c r="Q4" s="167"/>
+      <c r="R4" s="165" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="164"/>
-      <c r="T4" s="164"/>
-      <c r="U4" s="164"/>
-      <c r="V4" s="164"/>
-      <c r="W4" s="164"/>
-      <c r="X4" s="165"/>
-      <c r="Y4" s="163" t="str">
+      <c r="S4" s="166"/>
+      <c r="T4" s="166"/>
+      <c r="U4" s="166"/>
+      <c r="V4" s="166"/>
+      <c r="W4" s="166"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="165" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="164"/>
-      <c r="AA4" s="164"/>
-      <c r="AB4" s="164"/>
-      <c r="AC4" s="164"/>
-      <c r="AD4" s="164"/>
-      <c r="AE4" s="165"/>
-      <c r="AF4" s="163" t="str">
+      <c r="Z4" s="166"/>
+      <c r="AA4" s="166"/>
+      <c r="AB4" s="166"/>
+      <c r="AC4" s="166"/>
+      <c r="AD4" s="166"/>
+      <c r="AE4" s="167"/>
+      <c r="AF4" s="165" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="164"/>
-      <c r="AH4" s="164"/>
-      <c r="AI4" s="164"/>
-      <c r="AJ4" s="164"/>
-      <c r="AK4" s="164"/>
-      <c r="AL4" s="165"/>
-      <c r="AM4" s="163" t="str">
+      <c r="AG4" s="166"/>
+      <c r="AH4" s="166"/>
+      <c r="AI4" s="166"/>
+      <c r="AJ4" s="166"/>
+      <c r="AK4" s="166"/>
+      <c r="AL4" s="167"/>
+      <c r="AM4" s="165" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="164"/>
-      <c r="AO4" s="164"/>
-      <c r="AP4" s="164"/>
-      <c r="AQ4" s="164"/>
-      <c r="AR4" s="164"/>
-      <c r="AS4" s="165"/>
-      <c r="AT4" s="163" t="str">
+      <c r="AN4" s="166"/>
+      <c r="AO4" s="166"/>
+      <c r="AP4" s="166"/>
+      <c r="AQ4" s="166"/>
+      <c r="AR4" s="166"/>
+      <c r="AS4" s="167"/>
+      <c r="AT4" s="165" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="164"/>
-      <c r="AV4" s="164"/>
-      <c r="AW4" s="164"/>
-      <c r="AX4" s="164"/>
-      <c r="AY4" s="164"/>
-      <c r="AZ4" s="165"/>
-      <c r="BA4" s="163" t="str">
+      <c r="AU4" s="166"/>
+      <c r="AV4" s="166"/>
+      <c r="AW4" s="166"/>
+      <c r="AX4" s="166"/>
+      <c r="AY4" s="166"/>
+      <c r="AZ4" s="167"/>
+      <c r="BA4" s="165" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="164"/>
-      <c r="BC4" s="164"/>
-      <c r="BD4" s="164"/>
-      <c r="BE4" s="164"/>
-      <c r="BF4" s="164"/>
-      <c r="BG4" s="165"/>
-      <c r="BH4" s="163" t="str">
+      <c r="BB4" s="166"/>
+      <c r="BC4" s="166"/>
+      <c r="BD4" s="166"/>
+      <c r="BE4" s="166"/>
+      <c r="BF4" s="166"/>
+      <c r="BG4" s="167"/>
+      <c r="BH4" s="165" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="164"/>
-      <c r="BJ4" s="164"/>
-      <c r="BK4" s="164"/>
-      <c r="BL4" s="164"/>
-      <c r="BM4" s="164"/>
-      <c r="BN4" s="165"/>
+      <c r="BI4" s="166"/>
+      <c r="BJ4" s="166"/>
+      <c r="BK4" s="166"/>
+      <c r="BL4" s="166"/>
+      <c r="BM4" s="166"/>
+      <c r="BN4" s="167"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="109"/>
       <c r="B5" s="113" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
+      <c r="C5" s="164"/>
+      <c r="D5" s="164"/>
+      <c r="E5" s="164"/>
       <c r="F5" s="112"/>
       <c r="G5" s="112"/>
       <c r="H5" s="112"/>
       <c r="I5" s="112"/>
       <c r="J5" s="49"/>
-      <c r="K5" s="166">
+      <c r="K5" s="169">
         <f>K6</f>
         <v>44116</v>
       </c>
-      <c r="L5" s="167"/>
-      <c r="M5" s="167"/>
-      <c r="N5" s="167"/>
-      <c r="O5" s="167"/>
-      <c r="P5" s="167"/>
-      <c r="Q5" s="168"/>
-      <c r="R5" s="166">
+      <c r="L5" s="170"/>
+      <c r="M5" s="170"/>
+      <c r="N5" s="170"/>
+      <c r="O5" s="170"/>
+      <c r="P5" s="170"/>
+      <c r="Q5" s="171"/>
+      <c r="R5" s="169">
         <f>R6</f>
         <v>44123</v>
       </c>
-      <c r="S5" s="167"/>
-      <c r="T5" s="167"/>
-      <c r="U5" s="167"/>
-      <c r="V5" s="167"/>
-      <c r="W5" s="167"/>
-      <c r="X5" s="168"/>
-      <c r="Y5" s="166">
+      <c r="S5" s="170"/>
+      <c r="T5" s="170"/>
+      <c r="U5" s="170"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
+      <c r="X5" s="171"/>
+      <c r="Y5" s="169">
         <f>Y6</f>
         <v>44130</v>
       </c>
-      <c r="Z5" s="167"/>
-      <c r="AA5" s="167"/>
-      <c r="AB5" s="167"/>
-      <c r="AC5" s="167"/>
-      <c r="AD5" s="167"/>
-      <c r="AE5" s="168"/>
-      <c r="AF5" s="166">
+      <c r="Z5" s="170"/>
+      <c r="AA5" s="170"/>
+      <c r="AB5" s="170"/>
+      <c r="AC5" s="170"/>
+      <c r="AD5" s="170"/>
+      <c r="AE5" s="171"/>
+      <c r="AF5" s="169">
         <f>AF6</f>
         <v>44137</v>
       </c>
-      <c r="AG5" s="167"/>
-      <c r="AH5" s="167"/>
-      <c r="AI5" s="167"/>
-      <c r="AJ5" s="167"/>
-      <c r="AK5" s="167"/>
-      <c r="AL5" s="168"/>
-      <c r="AM5" s="166">
+      <c r="AG5" s="170"/>
+      <c r="AH5" s="170"/>
+      <c r="AI5" s="170"/>
+      <c r="AJ5" s="170"/>
+      <c r="AK5" s="170"/>
+      <c r="AL5" s="171"/>
+      <c r="AM5" s="169">
         <f>AM6</f>
         <v>44144</v>
       </c>
-      <c r="AN5" s="167"/>
-      <c r="AO5" s="167"/>
-      <c r="AP5" s="167"/>
-      <c r="AQ5" s="167"/>
-      <c r="AR5" s="167"/>
-      <c r="AS5" s="168"/>
-      <c r="AT5" s="166">
+      <c r="AN5" s="170"/>
+      <c r="AO5" s="170"/>
+      <c r="AP5" s="170"/>
+      <c r="AQ5" s="170"/>
+      <c r="AR5" s="170"/>
+      <c r="AS5" s="171"/>
+      <c r="AT5" s="169">
         <f>AT6</f>
         <v>44151</v>
       </c>
-      <c r="AU5" s="167"/>
-      <c r="AV5" s="167"/>
-      <c r="AW5" s="167"/>
-      <c r="AX5" s="167"/>
-      <c r="AY5" s="167"/>
-      <c r="AZ5" s="168"/>
-      <c r="BA5" s="166">
+      <c r="AU5" s="170"/>
+      <c r="AV5" s="170"/>
+      <c r="AW5" s="170"/>
+      <c r="AX5" s="170"/>
+      <c r="AY5" s="170"/>
+      <c r="AZ5" s="171"/>
+      <c r="BA5" s="169">
         <f>BA6</f>
         <v>44158</v>
       </c>
-      <c r="BB5" s="167"/>
-      <c r="BC5" s="167"/>
-      <c r="BD5" s="167"/>
-      <c r="BE5" s="167"/>
-      <c r="BF5" s="167"/>
-      <c r="BG5" s="168"/>
-      <c r="BH5" s="166">
+      <c r="BB5" s="170"/>
+      <c r="BC5" s="170"/>
+      <c r="BD5" s="170"/>
+      <c r="BE5" s="170"/>
+      <c r="BF5" s="170"/>
+      <c r="BG5" s="171"/>
+      <c r="BH5" s="169">
         <f>BH6</f>
         <v>44165</v>
       </c>
-      <c r="BI5" s="167"/>
-      <c r="BJ5" s="167"/>
-      <c r="BK5" s="167"/>
-      <c r="BL5" s="167"/>
-      <c r="BM5" s="167"/>
-      <c r="BN5" s="168"/>
+      <c r="BI5" s="170"/>
+      <c r="BJ5" s="170"/>
+      <c r="BK5" s="170"/>
+      <c r="BL5" s="170"/>
+      <c r="BM5" s="170"/>
+      <c r="BN5" s="171"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="48"/>
@@ -5492,11 +5492,11 @@
       </c>
       <c r="D19" s="126"/>
       <c r="E19" s="99">
-        <v>44118</v>
+        <v>44127</v>
       </c>
       <c r="F19" s="100">
         <f t="shared" si="6"/>
-        <v>44121</v>
+        <v>44130</v>
       </c>
       <c r="G19" s="61">
         <v>4</v>
@@ -5506,7 +5506,7 @@
       </c>
       <c r="I19" s="63">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J19" s="94"/>
       <c r="K19" s="106"/>
@@ -5576,11 +5576,11 @@
       </c>
       <c r="D20" s="126"/>
       <c r="E20" s="99">
-        <v>44119</v>
+        <v>44129</v>
       </c>
       <c r="F20" s="100">
         <f t="shared" si="6"/>
-        <v>44132</v>
+        <v>44142</v>
       </c>
       <c r="G20" s="61">
         <v>14</v>
@@ -5660,11 +5660,11 @@
       </c>
       <c r="D21" s="126"/>
       <c r="E21" s="99">
-        <v>44123</v>
+        <v>44131</v>
       </c>
       <c r="F21" s="100">
         <f t="shared" si="6"/>
-        <v>44125</v>
+        <v>44133</v>
       </c>
       <c r="G21" s="61">
         <v>3</v>
@@ -5744,11 +5744,11 @@
       </c>
       <c r="D22" s="126"/>
       <c r="E22" s="99">
-        <v>44152</v>
+        <v>44136</v>
       </c>
       <c r="F22" s="100">
         <f t="shared" si="6"/>
-        <v>44157</v>
+        <v>44141</v>
       </c>
       <c r="G22" s="61">
         <v>6</v>
@@ -5758,7 +5758,7 @@
       </c>
       <c r="I22" s="63">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J22" s="94"/>
       <c r="K22" s="106"/>
@@ -5828,11 +5828,11 @@
       </c>
       <c r="D23" s="126"/>
       <c r="E23" s="99">
-        <v>44160</v>
+        <v>44137</v>
       </c>
       <c r="F23" s="100">
         <f t="shared" si="6"/>
-        <v>44166</v>
+        <v>44143</v>
       </c>
       <c r="G23" s="61">
         <v>7</v>
@@ -5990,11 +5990,11 @@
       </c>
       <c r="D25" s="126"/>
       <c r="E25" s="99">
-        <v>44126</v>
+        <v>44129</v>
       </c>
       <c r="F25" s="100">
         <f t="shared" si="6"/>
-        <v>44129</v>
+        <v>44132</v>
       </c>
       <c r="G25" s="61">
         <v>4</v>
@@ -6004,7 +6004,7 @@
       </c>
       <c r="I25" s="63">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J25" s="94"/>
       <c r="K25" s="106"/>
@@ -6319,9 +6319,7 @@
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.5</v>
       </c>
-      <c r="B29" s="125" t="s">
-        <v>10</v>
-      </c>
+      <c r="B29" s="125"/>
       <c r="D29" s="126"/>
       <c r="E29" s="99">
         <v>43154</v>
@@ -7566,15 +7564,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7585,6 +7574,15 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H43">

</xml_diff>